<commit_message>
l2 pca opt rank
</commit_message>
<xml_diff>
--- a/CancerDT.xlsx
+++ b/CancerDT.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\CancerAceFiltering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75A1C355-2D8E-4BD8-8895-624FE688E0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBE92E3-0204-4BAC-8F3C-A25B1294F28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D6E6FFAA-0B19-433F-BE05-56A6616BA0F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{D6E6FFAA-0B19-433F-BE05-56A6616BA0F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="DT 20%" sheetId="1" r:id="rId1"/>
+    <sheet name="DT 20%" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="DT_0%_rank5" sheetId="7" state="hidden" r:id="rId2"/>
+    <sheet name="DT_0%_rank8" sheetId="6" r:id="rId3"/>
+    <sheet name="DT_10%_rank8" sheetId="4" r:id="rId4"/>
+    <sheet name="DT_20%_rank8" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>---------split 1 --------------------</t>
   </si>
@@ -84,12 +88,83 @@
   <si>
     <t>---------split 10 --------------------</t>
   </si>
+  <si>
+    <t>PREDICTED</t>
+  </si>
+  <si>
+    <t>benign</t>
+  </si>
+  <si>
+    <t>malignant</t>
+  </si>
+  <si>
+    <t>SVM with without  Data Curation</t>
+  </si>
+  <si>
+    <t>SVM with with Training  Data Curation</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Prob of False Alarm</t>
+  </si>
+  <si>
+    <r>
+      <t>tree_model = DecisionTreeClassifier(max_depth=depth,random_state=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,criterion=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"gini"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>max_depth=depth,random_state=22,criterion="entropy",min_samples_split = 5</t>
+  </si>
+  <si>
+    <t>DT on raw data</t>
+  </si>
+  <si>
+    <t>DT on Curated Data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +196,32 @@
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF098156"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFA31515"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +252,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -278,20 +383,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -312,7 +536,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,283 +952,283 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14A47B-EE7D-4598-91C5-8A4199D0F3DA}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>4.88</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>4.3899999999999997</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <f>B3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="10">
         <f>SUM(C3,C13,C23,C33,C43,C53,C63,C73,C83,C93)/10</f>
         <v>5.6099999999999994</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="10">
         <f>SUM(D3,D13,D23,D33,D43,D53,D63,D73,D83,D93)/10</f>
         <v>4.6330000000000009</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13">
+      <c r="I3" s="10"/>
+      <c r="J3" s="11">
         <f>(H3-G3)/H3*100</f>
         <v>-21.087848046622025</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="10">
-        <v>2</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
         <v>3.41</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>4.3899999999999997</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <f t="shared" ref="F4:F10" si="0">B4</f>
         <v>2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <f t="shared" ref="G4:H10" si="1">SUM(C4,C14,C24,C34,C44,C54,C64,C74,C84,C94)/10</f>
         <v>5.6589999999999989</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <f t="shared" si="1"/>
         <v>5.1219999999999999</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="11">
         <f t="shared" ref="J4:J10" si="2">(H4-G4)/H4*100</f>
         <v>-10.484185864896507</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="10">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
         <v>5</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>3.41</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>2.93</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="10">
         <f t="shared" si="1"/>
         <v>5.1219999999999999</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <f t="shared" si="1"/>
         <v>4.3899999999999997</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="11">
         <f t="shared" si="2"/>
         <v>-16.6742596810934</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>10</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>4.3899999999999997</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>2.44</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <f t="shared" si="1"/>
         <v>6.2919999999999998</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <f t="shared" si="1"/>
         <v>5.8049999999999997</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="11">
         <f t="shared" si="2"/>
         <v>-8.389319552110253</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>20</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>2.44</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>3.9</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="10">
         <f t="shared" si="1"/>
         <v>4.4879999999999995</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <f t="shared" si="1"/>
         <v>5.9009999999999998</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="12">
         <f t="shared" si="2"/>
         <v>23.945094051855623</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>30</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>2.93</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>2.93</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <f t="shared" si="1"/>
         <v>7.169999999999999</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="12">
         <f t="shared" si="2"/>
         <v>16.317991631799153</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>40</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>15.12</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>13.66</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="10">
         <f t="shared" si="1"/>
         <v>8.5350000000000001</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <f t="shared" si="1"/>
         <v>10.291999999999998</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="12">
         <f t="shared" si="2"/>
         <v>17.071511853867065</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>50</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>13.66</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>23.9</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <f t="shared" si="1"/>
         <v>31.463000000000001</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <f t="shared" si="1"/>
         <v>26.78</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="11">
         <f t="shared" si="2"/>
         <v>-17.486930545182972</v>
       </c>
@@ -916,126 +1239,126 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>0</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="8">
         <v>0</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <v>6.83</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="10">
-        <v>2</v>
-      </c>
-      <c r="C14" s="10">
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
         <v>6.83</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="8">
         <v>7.32</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="9">
-        <v>2</v>
-      </c>
-      <c r="B15" s="10">
+      <c r="A15" s="7">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8">
         <v>5</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <v>6.83</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="8">
         <v>8.7799999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="8">
         <v>10</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>8.2899999999999991</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="8">
         <v>7.32</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>4</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="8">
         <v>20</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>7.8</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="8">
         <v>9.27</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="9">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="8">
         <v>30</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>8.2899999999999991</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>6</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <v>40</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>8.7799999999999994</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>7.8</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="9">
+      <c r="A20" s="7">
         <v>7</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <v>50</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>36.590000000000003</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="8">
         <v>21.46</v>
       </c>
     </row>
@@ -1045,126 +1368,126 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="9">
+      <c r="A23" s="7">
         <v>0</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="8">
         <v>0</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="8">
         <v>5.37</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9">
+      <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B24" s="10">
-        <v>2</v>
-      </c>
-      <c r="C24" s="10">
+      <c r="B24" s="8">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8">
         <v>5.37</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9">
-        <v>2</v>
-      </c>
-      <c r="B25" s="10">
+      <c r="A25" s="7">
+        <v>2</v>
+      </c>
+      <c r="B25" s="8">
         <v>5</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="8">
         <v>5.37</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="8">
         <v>2.44</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="9">
+      <c r="A26" s="7">
         <v>3</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>10</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="8">
         <v>4.88</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>4</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="8">
         <v>20</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="8">
         <v>3.9</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="9">
+      <c r="A28" s="7">
         <v>5</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>30</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="8">
         <v>6.83</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="8">
         <v>9.27</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="9">
+      <c r="A29" s="7">
         <v>6</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="8">
         <v>40</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="8">
         <v>4.88</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="8">
         <v>7.32</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="9">
+      <c r="A30" s="7">
         <v>7</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="8">
         <v>50</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="8">
         <v>30.24</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="8">
         <v>31.22</v>
       </c>
     </row>
@@ -1174,126 +1497,126 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="9">
+      <c r="A33" s="7">
         <v>0</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="8">
         <v>0</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="8">
         <v>5.37</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="9">
+      <c r="A34" s="7">
         <v>1</v>
       </c>
-      <c r="B34" s="10">
-        <v>2</v>
-      </c>
-      <c r="C34" s="10">
+      <c r="B34" s="8">
+        <v>2</v>
+      </c>
+      <c r="C34" s="8">
         <v>5.37</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="8">
         <v>6.34</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="9">
-        <v>2</v>
-      </c>
-      <c r="B35" s="10">
+      <c r="A35" s="7">
+        <v>2</v>
+      </c>
+      <c r="B35" s="8">
         <v>5</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="8">
         <v>4.3899999999999997</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="9">
+      <c r="A36" s="7">
         <v>3</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="8">
         <v>10</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="8">
         <v>5.85</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="9">
+      <c r="A37" s="7">
         <v>4</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="8">
         <v>20</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="8">
         <v>4.3899999999999997</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="9">
+      <c r="A38" s="7">
         <v>5</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="8">
         <v>30</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="8">
         <v>7.8</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="8">
         <v>10.24</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="9">
+      <c r="A39" s="7">
         <v>6</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="8">
         <v>40</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="8">
         <v>3.9</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="8">
         <v>8.2899999999999991</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="9">
+      <c r="A40" s="7">
         <v>7</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="8">
         <v>50</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="8">
         <v>14.63</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="8">
         <v>42.44</v>
       </c>
     </row>
@@ -1303,126 +1626,126 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2">
         <v>1</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="9">
+      <c r="A43" s="7">
         <v>0</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="8">
         <v>0</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="8">
         <v>3.9</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="8">
         <v>2.93</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="9">
+      <c r="A44" s="7">
         <v>1</v>
       </c>
-      <c r="B44" s="10">
-        <v>2</v>
-      </c>
-      <c r="C44" s="10">
+      <c r="B44" s="8">
+        <v>2</v>
+      </c>
+      <c r="C44" s="8">
         <v>4.88</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="8">
         <v>4.88</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="9">
-        <v>2</v>
-      </c>
-      <c r="B45" s="10">
+      <c r="A45" s="7">
+        <v>2</v>
+      </c>
+      <c r="B45" s="8">
         <v>5</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="8">
         <v>4.88</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="9">
+      <c r="A46" s="7">
         <v>3</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="8">
         <v>10</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="8">
         <v>5.85</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="9">
+      <c r="A47" s="7">
         <v>4</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="8">
         <v>20</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="8">
         <v>4.88</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="9">
+      <c r="A48" s="7">
         <v>5</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="8">
         <v>30</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="8">
         <v>5.37</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="9">
+      <c r="A49" s="7">
         <v>6</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="8">
         <v>40</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="8">
         <v>5.37</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="8">
         <v>5.37</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="9">
+      <c r="A50" s="7">
         <v>7</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="8">
         <v>50</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="8">
         <v>17.07</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="8">
         <v>30.24</v>
       </c>
     </row>
@@ -1432,126 +1755,126 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="4">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="9">
+      <c r="A53" s="7">
         <v>0</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="8">
         <v>0</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="8">
         <v>6.34</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="9">
+      <c r="A54" s="7">
         <v>1</v>
       </c>
-      <c r="B54" s="10">
-        <v>2</v>
-      </c>
-      <c r="C54" s="10">
+      <c r="B54" s="8">
+        <v>2</v>
+      </c>
+      <c r="C54" s="8">
         <v>4.88</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="9">
-        <v>2</v>
-      </c>
-      <c r="B55" s="10">
+      <c r="A55" s="7">
+        <v>2</v>
+      </c>
+      <c r="B55" s="8">
         <v>5</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="8">
         <v>4.88</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="8">
         <v>3.9</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="9">
+      <c r="A56" s="7">
         <v>3</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="8">
         <v>10</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="8">
         <v>7.32</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="8">
         <v>6.34</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="9">
+      <c r="A57" s="7">
         <v>4</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="8">
         <v>20</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="8">
         <v>3.9</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="8">
         <v>3.9</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="9">
+      <c r="A58" s="7">
         <v>5</v>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="8">
         <v>30</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="8">
         <v>5.85</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="9">
+      <c r="A59" s="7">
         <v>6</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B59" s="8">
         <v>40</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="8">
         <v>10.24</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="8">
         <v>16.100000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="9">
+      <c r="A60" s="7">
         <v>7</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="8">
         <v>50</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="8">
         <v>53.17</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="8">
         <v>45.37</v>
       </c>
     </row>
@@ -1561,126 +1884,126 @@
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" s="4">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="2">
         <v>1</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="9">
+      <c r="A63" s="7">
         <v>0</v>
       </c>
-      <c r="B63" s="10">
+      <c r="B63" s="8">
         <v>0</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="8">
         <v>5.85</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="9">
+      <c r="A64" s="7">
         <v>1</v>
       </c>
-      <c r="B64" s="10">
-        <v>2</v>
-      </c>
-      <c r="C64" s="10">
+      <c r="B64" s="8">
+        <v>2</v>
+      </c>
+      <c r="C64" s="8">
         <v>5.85</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="9">
-        <v>2</v>
-      </c>
-      <c r="B65" s="10">
+      <c r="A65" s="7">
+        <v>2</v>
+      </c>
+      <c r="B65" s="8">
         <v>5</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="8">
         <v>5.37</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="8">
         <v>5.85</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="9">
+      <c r="A66" s="7">
         <v>3</v>
       </c>
-      <c r="B66" s="10">
+      <c r="B66" s="8">
         <v>10</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="8">
         <v>7.32</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="8">
         <v>6.34</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="9">
+      <c r="A67" s="7">
         <v>4</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="8">
         <v>20</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="8">
         <v>5.37</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="8">
         <v>6.34</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="9">
+      <c r="A68" s="7">
         <v>5</v>
       </c>
-      <c r="B68" s="10">
+      <c r="B68" s="8">
         <v>30</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="8">
         <v>5.37</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="8">
         <v>6.34</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="9">
+      <c r="A69" s="7">
         <v>6</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="8">
         <v>40</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="8">
         <v>8.2899999999999991</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="8">
         <v>13.66</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="9">
+      <c r="A70" s="7">
         <v>7</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B70" s="8">
         <v>50</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="8">
         <v>24.88</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="8">
         <v>19.510000000000002</v>
       </c>
     </row>
@@ -1690,126 +2013,126 @@
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" s="4">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="2">
         <v>1</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D72" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="9">
+      <c r="A73" s="7">
         <v>0</v>
       </c>
-      <c r="B73" s="10">
+      <c r="B73" s="8">
         <v>0</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="8">
         <v>5.85</v>
       </c>
-      <c r="D73" s="10">
+      <c r="D73" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="9">
+      <c r="A74" s="7">
         <v>1</v>
       </c>
-      <c r="B74" s="10">
-        <v>2</v>
-      </c>
-      <c r="C74" s="10">
+      <c r="B74" s="8">
+        <v>2</v>
+      </c>
+      <c r="C74" s="8">
         <v>6.34</v>
       </c>
-      <c r="D74" s="10">
+      <c r="D74" s="8">
         <v>5.37</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="9">
-        <v>2</v>
-      </c>
-      <c r="B75" s="10">
+      <c r="A75" s="7">
+        <v>2</v>
+      </c>
+      <c r="B75" s="8">
         <v>5</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="8">
         <v>6.34</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="9">
+      <c r="A76" s="7">
         <v>3</v>
       </c>
-      <c r="B76" s="10">
+      <c r="B76" s="8">
         <v>10</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="8">
         <v>8.2899999999999991</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="8">
         <v>4.88</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="9">
+      <c r="A77" s="7">
         <v>4</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="8">
         <v>20</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="8">
         <v>5.37</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D77" s="8">
         <v>8.2899999999999991</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="9">
+      <c r="A78" s="7">
         <v>5</v>
       </c>
-      <c r="B78" s="10">
+      <c r="B78" s="8">
         <v>30</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="8">
         <v>4.88</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D78" s="8">
         <v>8.7799999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="9">
+      <c r="A79" s="7">
         <v>6</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" s="8">
         <v>40</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="8">
         <v>14.63</v>
       </c>
-      <c r="D79" s="10">
+      <c r="D79" s="8">
         <v>14.63</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="9">
+      <c r="A80" s="7">
         <v>7</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="8">
         <v>50</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="8">
         <v>57.56</v>
       </c>
-      <c r="D80" s="10">
+      <c r="D80" s="8">
         <v>20</v>
       </c>
     </row>
@@ -1819,126 +2142,126 @@
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C82" s="4">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="2">
         <v>1</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D82" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="9">
+      <c r="A83" s="7">
         <v>0</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="8">
         <v>0</v>
       </c>
-      <c r="C83" s="10">
+      <c r="C83" s="8">
         <v>5.37</v>
       </c>
-      <c r="D83" s="10">
+      <c r="D83" s="8">
         <v>3.41</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="9">
+      <c r="A84" s="7">
         <v>1</v>
       </c>
-      <c r="B84" s="10">
-        <v>2</v>
-      </c>
-      <c r="C84" s="10">
+      <c r="B84" s="8">
+        <v>2</v>
+      </c>
+      <c r="C84" s="8">
         <v>7.32</v>
       </c>
-      <c r="D84" s="10">
+      <c r="D84" s="8">
         <v>3.9</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="9">
-        <v>2</v>
-      </c>
-      <c r="B85" s="10">
+      <c r="A85" s="7">
+        <v>2</v>
+      </c>
+      <c r="B85" s="8">
         <v>5</v>
       </c>
-      <c r="C85" s="10">
+      <c r="C85" s="8">
         <v>5.85</v>
       </c>
-      <c r="D85" s="10">
+      <c r="D85" s="8">
         <v>2.93</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="9">
+      <c r="A86" s="7">
         <v>3</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" s="8">
         <v>10</v>
       </c>
-      <c r="C86" s="10">
+      <c r="C86" s="8">
         <v>4.88</v>
       </c>
-      <c r="D86" s="10">
+      <c r="D86" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="9">
+      <c r="A87" s="7">
         <v>4</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" s="8">
         <v>20</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="8">
         <v>2.93</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D87" s="8">
         <v>3.41</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="9">
+      <c r="A88" s="7">
         <v>5</v>
       </c>
-      <c r="B88" s="10">
+      <c r="B88" s="8">
         <v>30</v>
       </c>
-      <c r="C88" s="10">
+      <c r="C88" s="8">
         <v>3.41</v>
       </c>
-      <c r="D88" s="10">
+      <c r="D88" s="8">
         <v>7.8</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="9">
+      <c r="A89" s="7">
         <v>6</v>
       </c>
-      <c r="B89" s="10">
+      <c r="B89" s="8">
         <v>40</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="8">
         <v>5.85</v>
       </c>
-      <c r="D89" s="10">
+      <c r="D89" s="8">
         <v>7.8</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="9">
+      <c r="A90" s="7">
         <v>7</v>
       </c>
-      <c r="B90" s="10">
+      <c r="B90" s="8">
         <v>50</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="8">
         <v>27.32</v>
       </c>
-      <c r="D90" s="10">
+      <c r="D90" s="8">
         <v>15.61</v>
       </c>
     </row>
@@ -1948,126 +2271,126 @@
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C92" s="4">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="2">
         <v>1</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D92" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="9">
+      <c r="A93" s="7">
         <v>0</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B93" s="8">
         <v>0</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C93" s="8">
         <v>6.34</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D93" s="8">
         <v>3.9</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="9">
+      <c r="A94" s="7">
         <v>1</v>
       </c>
-      <c r="B94" s="10">
-        <v>2</v>
-      </c>
-      <c r="C94" s="10">
+      <c r="B94" s="8">
+        <v>2</v>
+      </c>
+      <c r="C94" s="8">
         <v>6.34</v>
       </c>
-      <c r="D94" s="10">
+      <c r="D94" s="8">
         <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="9">
-        <v>2</v>
-      </c>
-      <c r="B95" s="10">
+      <c r="A95" s="7">
+        <v>2</v>
+      </c>
+      <c r="B95" s="8">
         <v>5</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C95" s="8">
         <v>3.9</v>
       </c>
-      <c r="D95" s="10">
+      <c r="D95" s="8">
         <v>3.9</v>
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="9">
+      <c r="A96" s="7">
         <v>3</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B96" s="8">
         <v>10</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C96" s="8">
         <v>5.85</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D96" s="8">
         <v>5.37</v>
       </c>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="9">
+      <c r="A97" s="7">
         <v>4</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="8">
         <v>20</v>
       </c>
-      <c r="C97" s="10">
+      <c r="C97" s="8">
         <v>3.9</v>
       </c>
-      <c r="D97" s="10">
+      <c r="D97" s="8">
         <v>5.37</v>
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="9">
+      <c r="A98" s="7">
         <v>5</v>
       </c>
-      <c r="B98" s="10">
+      <c r="B98" s="8">
         <v>30</v>
       </c>
-      <c r="C98" s="10">
+      <c r="C98" s="8">
         <v>9.27</v>
       </c>
-      <c r="D98" s="10">
+      <c r="D98" s="8">
         <v>6.83</v>
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="9">
+      <c r="A99" s="7">
         <v>6</v>
       </c>
-      <c r="B99" s="10">
+      <c r="B99" s="8">
         <v>40</v>
       </c>
-      <c r="C99" s="10">
+      <c r="C99" s="8">
         <v>8.2899999999999991</v>
       </c>
-      <c r="D99" s="10">
+      <c r="D99" s="8">
         <v>8.2899999999999991</v>
       </c>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="9">
+      <c r="A100" s="7">
         <v>7</v>
       </c>
-      <c r="B100" s="10">
+      <c r="B100" s="8">
         <v>50</v>
       </c>
-      <c r="C100" s="10">
+      <c r="C100" s="8">
         <v>39.51</v>
       </c>
-      <c r="D100" s="10">
+      <c r="D100" s="8">
         <v>18.05</v>
       </c>
     </row>
@@ -2078,4 +2401,603 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B81578-E6ED-4831-97E7-CB04D93B811C}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="33.77734375" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="33.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.95982100000000004</v>
+      </c>
+      <c r="D4" s="20">
+        <v>4.0178999999999999E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.94419600000000004</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5.5803999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="36"/>
+      <c r="B5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>7.0821999999999996E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.92917799999999995</v>
+      </c>
+      <c r="E5" s="22">
+        <v>4.1076000000000001E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.958924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39">
+        <v>0.92917799999999995</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="29">
+        <v>0.958924</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29">
+        <v>4.0178999999999999E-2</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="29">
+        <v>5.5803999999999999E-2</v>
+      </c>
+      <c r="F8" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A8CAB9-F611-4F2A-9B90-91F7C0D0FFBF}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.95610099999999998</v>
+      </c>
+      <c r="D4" s="20">
+        <v>4.3899000000000001E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.95610099999999998</v>
+      </c>
+      <c r="F4" s="20">
+        <v>4.3899000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="36"/>
+      <c r="B5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>6.5156000000000006E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.93484</v>
+      </c>
+      <c r="E5" s="22">
+        <v>4.3908999999999997E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.95609100000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39">
+        <v>0.93484</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="29">
+        <v>0.95609100000000002</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="39">
+        <v>4.3899000000000001E-2</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="29">
+        <v>4.3899000000000001E-2</v>
+      </c>
+      <c r="F8" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDF2732-A88A-4598-96CB-EBBFD2E03CFF}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.94419600000000004</v>
+      </c>
+      <c r="D4" s="20">
+        <v>5.5803999999999999E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.94866099999999998</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5.1339000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="46"/>
+      <c r="B5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>8.6402000000000007E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.91359800000000002</v>
+      </c>
+      <c r="E5" s="22">
+        <v>5.8074000000000001E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.94192600000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="39">
+        <v>0.91359800000000002</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="39">
+        <v>0.94192600000000004</v>
+      </c>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="39">
+        <v>5.5803999999999999E-2</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="39">
+        <v>5.1339000000000003E-2</v>
+      </c>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660E2B60-68B3-4D29-919F-CB6316E5A518}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.94121999999999995</v>
+      </c>
+      <c r="D4" s="20">
+        <v>5.8779999999999999E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.94047599999999998</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5.9524000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="36"/>
+      <c r="B5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.11898</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.88102000000000003</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.109065</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.89093500000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="29">
+        <v>0.88102000000000003</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="29">
+        <v>0.89093500000000003</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29">
+        <v>5.8779999999999999E-2</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="29">
+        <v>5.9524000000000001E-2</v>
+      </c>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>